<commit_message>
TE consideration of DHW generation type/system is considered for calculation of DHW
TE pre processing
and
annualSimulation

+ Dummy data TE

-> recalculated with DHW for TE data
</commit_message>
<xml_diff>
--- a/data_preprocessing/tiefenerhebung/TE_data/#Alle_Daten_DB_TE_inkl_TEK_GEO_Dummy.xlsx
+++ b/data_preprocessing/tiefenerhebung/TE_data/#Alle_Daten_DB_TE_inkl_TEK_GEO_Dummy.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="24228"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="25128"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\julia\Desktop\DIBS---Dynamic-ISO-Building-Simulator-master\data_preprocessing\tiefenerhebung\TE_data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\julia\Desktop\DIBS---Dynamic-ISO-Building-Simulator\data_preprocessing\tiefenerhebung\TE_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{9E0BDDA2-BB4B-4D52-A861-BA8EF2D3283D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{72869D32-3CE2-4A49-AE36-D288E9700630}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1050" yWindow="-120" windowWidth="27870" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2356" uniqueCount="924">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2377" uniqueCount="928">
   <si>
     <t>pr_var_name</t>
   </si>
@@ -2792,6 +2792,18 @@
   </si>
   <si>
     <t>AB123456_0_20</t>
+  </si>
+  <si>
+    <t>bp_ww_gen_1</t>
+  </si>
+  <si>
+    <t>zentraler Wärmeerzeuger</t>
+  </si>
+  <si>
+    <t>el. Durchlauferhitzer</t>
+  </si>
+  <si>
+    <t>el. Kleinspeicher</t>
   </si>
 </sst>
 </file>
@@ -2850,11 +2862,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -3193,18 +3206,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:ADO21"/>
+  <dimension ref="A1:ADP21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A22" sqref="A22:XFD51"/>
+    <sheetView tabSelected="1" topLeftCell="ACQ1" workbookViewId="0">
+      <selection activeCell="ADP1" sqref="ADP1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="29.7109375" customWidth="1"/>
+    <col min="796" max="796" width="13.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:795" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:796" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -5590,8 +5604,11 @@
       <c r="ADO1" s="1" t="s">
         <v>794</v>
       </c>
+      <c r="ADP1" s="2" t="s">
+        <v>924</v>
+      </c>
     </row>
-    <row r="2" spans="1:795" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:796" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>904</v>
       </c>
@@ -6072,8 +6089,11 @@
       <c r="ADK2">
         <v>0</v>
       </c>
+      <c r="ADP2" t="s">
+        <v>925</v>
+      </c>
     </row>
-    <row r="3" spans="1:795" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:796" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>905</v>
       </c>
@@ -6449,8 +6469,11 @@
       <c r="ADK3">
         <v>0</v>
       </c>
+      <c r="ADP3" t="s">
+        <v>926</v>
+      </c>
     </row>
-    <row r="4" spans="1:795" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:796" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>906</v>
       </c>
@@ -6880,8 +6903,11 @@
       <c r="ADK4">
         <v>0</v>
       </c>
+      <c r="ADP4" t="s">
+        <v>927</v>
+      </c>
     </row>
-    <row r="5" spans="1:795" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:796" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>907</v>
       </c>
@@ -7281,8 +7307,11 @@
       <c r="ADK5">
         <v>0</v>
       </c>
+      <c r="ADP5" t="s">
+        <v>927</v>
+      </c>
     </row>
-    <row r="6" spans="1:795" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:796" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>908</v>
       </c>
@@ -7673,8 +7702,11 @@
       <c r="ADK6">
         <v>0</v>
       </c>
+      <c r="ADP6" t="s">
+        <v>927</v>
+      </c>
     </row>
-    <row r="7" spans="1:795" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:796" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>909</v>
       </c>
@@ -8101,8 +8133,11 @@
       <c r="ADK7">
         <v>0</v>
       </c>
+      <c r="ADP7" t="s">
+        <v>808</v>
+      </c>
     </row>
-    <row r="8" spans="1:795" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:796" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>910</v>
       </c>
@@ -8577,8 +8612,11 @@
       <c r="ADK8">
         <v>0</v>
       </c>
+      <c r="ADP8" t="s">
+        <v>925</v>
+      </c>
     </row>
-    <row r="9" spans="1:795" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:796" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>911</v>
       </c>
@@ -9032,8 +9070,11 @@
       <c r="ADK9">
         <v>0</v>
       </c>
+      <c r="ADP9" t="s">
+        <v>927</v>
+      </c>
     </row>
-    <row r="10" spans="1:795" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:796" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>912</v>
       </c>
@@ -9508,8 +9549,11 @@
       <c r="ADK10">
         <v>0</v>
       </c>
+      <c r="ADP10" t="s">
+        <v>927</v>
+      </c>
     </row>
-    <row r="11" spans="1:795" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:796" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>913</v>
       </c>
@@ -10029,8 +10073,11 @@
       <c r="ADK11">
         <v>0</v>
       </c>
+      <c r="ADP11" t="s">
+        <v>925</v>
+      </c>
     </row>
-    <row r="12" spans="1:795" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:796" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>914</v>
       </c>
@@ -10550,8 +10597,11 @@
       <c r="ADK12">
         <v>0</v>
       </c>
+      <c r="ADP12" t="s">
+        <v>927</v>
+      </c>
     </row>
-    <row r="13" spans="1:795" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:796" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>915</v>
       </c>
@@ -11164,8 +11214,11 @@
       <c r="ADK13">
         <v>0</v>
       </c>
+      <c r="ADP13" t="s">
+        <v>926</v>
+      </c>
     </row>
-    <row r="14" spans="1:795" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:796" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>916</v>
       </c>
@@ -11514,8 +11567,11 @@
       <c r="ADK14">
         <v>0</v>
       </c>
+      <c r="ADP14" t="s">
+        <v>927</v>
+      </c>
     </row>
-    <row r="15" spans="1:795" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:796" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>917</v>
       </c>
@@ -12035,8 +12091,11 @@
       <c r="ADK15">
         <v>0</v>
       </c>
+      <c r="ADP15" t="s">
+        <v>808</v>
+      </c>
     </row>
-    <row r="16" spans="1:795" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:796" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>918</v>
       </c>
@@ -12499,8 +12558,11 @@
       <c r="ADK16">
         <v>0</v>
       </c>
+      <c r="ADP16" t="s">
+        <v>925</v>
+      </c>
     </row>
-    <row r="17" spans="1:794" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:796" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>919</v>
       </c>
@@ -13122,8 +13184,11 @@
       <c r="ADN17">
         <v>2</v>
       </c>
+      <c r="ADP17" t="s">
+        <v>927</v>
+      </c>
     </row>
-    <row r="18" spans="1:794" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:796" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>920</v>
       </c>
@@ -13796,8 +13861,11 @@
       <c r="ADK18">
         <v>0</v>
       </c>
+      <c r="ADP18" t="s">
+        <v>927</v>
+      </c>
     </row>
-    <row r="19" spans="1:794" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:796" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>921</v>
       </c>
@@ -14281,8 +14349,11 @@
       <c r="ADK19">
         <v>0</v>
       </c>
+      <c r="ADP19" t="s">
+        <v>808</v>
+      </c>
     </row>
-    <row r="20" spans="1:794" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:796" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>922</v>
       </c>
@@ -14856,8 +14927,11 @@
       <c r="ADN20">
         <v>2</v>
       </c>
+      <c r="ADP20" t="s">
+        <v>925</v>
+      </c>
     </row>
-    <row r="21" spans="1:794" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:796" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>923</v>
       </c>
@@ -15214,9 +15288,13 @@
       </c>
       <c r="ADK21">
         <v>0</v>
+      </c>
+      <c r="ADP21" t="s">
+        <v>927</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>